<commit_message>
Relax Recipe Sheet Formatting Update
Minor format update
</commit_message>
<xml_diff>
--- a/Solution_recipes/DS_SS_Relax/Relax.xlsx
+++ b/Solution_recipes/DS_SS_Relax/Relax.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\Recipes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\GitHub\Protocols\Solution_recipes\DS_SS_Relax\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE49C66-A702-4AC4-AC72-FEB32E079837}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAA0B18-31D4-48A1-A2F2-A41E52A539DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$J$15</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
 </workbook>
@@ -109,9 +109,6 @@
     <t>Target pH = 7.00</t>
   </si>
   <si>
-    <t>HCl / KOH added</t>
-  </si>
-  <si>
     <t>Sigma
 (Roche)</t>
   </si>
@@ -125,6 +122,9 @@
   </si>
   <si>
     <t>Amount added (g)</t>
+  </si>
+  <si>
+    <t>Total HCl / KOH added</t>
   </si>
 </sst>
 </file>
@@ -171,7 +171,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -366,11 +366,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -399,9 +451,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -411,24 +460,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,6 +485,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -774,7 +838,7 @@
   <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection sqref="A1:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -793,10 +857,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -832,42 +896,42 @@
       <c r="G4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14">
         <v>74.55</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="14">
         <v>99.6</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="15">
         <f t="shared" ref="F5:F8" si="0">D5/(E5/100)</f>
         <v>74.849397590361448</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="16">
         <f>F5*0.1</f>
         <v>7.4849397590361448</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="16">
         <f t="shared" ref="I5:I8" si="1">H5/2</f>
         <v>3.7424698795180724</v>
       </c>
@@ -877,28 +941,28 @@
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14">
         <v>68.08</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="14">
         <v>97.9</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="15">
         <f t="shared" si="0"/>
         <v>69.540347293156273</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="16">
         <f>F6*0.02</f>
         <v>1.3908069458631256</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="16">
         <f t="shared" si="1"/>
         <v>0.69540347293156279</v>
       </c>
@@ -908,28 +972,28 @@
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14">
         <v>380.35</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="14">
         <v>97.9</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="15">
         <f t="shared" si="0"/>
         <v>388.50868232890701</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="16">
         <f>F7*0.002</f>
         <v>0.77701736465781401</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="16">
         <f t="shared" si="1"/>
         <v>0.38850868232890701</v>
       </c>
@@ -939,30 +1003,30 @@
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="20">
+      <c r="B8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="14">
         <v>55208921</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="18">
         <v>605.19000000000005</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="19">
         <v>99</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="15">
         <f t="shared" si="0"/>
         <v>611.30303030303037</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="16">
         <f>F8*0.004</f>
         <v>2.4452121212121214</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="16">
         <f t="shared" si="1"/>
         <v>1.2226060606060607</v>
       </c>
@@ -972,53 +1036,57 @@
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="26" t="s">
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="13"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="25"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="12"/>
+      <c r="B12" s="11"/>
     </row>
-    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="29"/>
     </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="13"/>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="31"/>
+    </row>
+    <row r="15" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
     </row>
     <row r="37" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="42" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -1046,22 +1114,18 @@
     <row r="72" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="73" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="95" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="94" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100965EA08FA511AE4C9FFF632E6536ED13" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abfa450e2c882fa05ec7f6a4b4016779">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a" xmlns:ns3="6cbc0c5a-d948-46e5-8624-1bad210f77c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53678093842f3275b6926b32e7a9c141" ns2:_="" ns3:_="">
     <xsd:import namespace="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
@@ -1284,7 +1348,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LabArchives xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <eid>MTkzLjcwMDAwMDAwMDAwMDAyfDY3MzMyMS8xNDkvRW50cnlQYXJ0LzEzNjcwOTU4NjB8NDkxLjc=</eid>
+  <version>35</version>
+  <updated-at>2023-05-23T19:13:43Z</updated-at>
+</LabArchives>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1293,32 +1371,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LabArchives xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <eid>MTkzLjcwMDAwMDAwMDAwMDAyfDY3MzMyMS8xNDkvRW50cnlQYXJ0LzEzNjcwOTU4NjB8NDkxLjc=</eid>
-  <version>35</version>
-  <updated-at>2023-05-23T19:13:43Z</updated-at>
-</LabArchives>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3012E31E-5C99-4C5B-9323-B5D42B3C4F74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7A5D5A9-477B-4B97-9F9B-D797D2834A6C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1337,18 +1390,35 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3012E31E-5C99-4C5B-9323-B5D42B3C4F74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33053450-05E7-49E1-931C-3F2FFF53B7FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{576E4525-D34E-471F-91EB-AF7A16356FDF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33053450-05E7-49E1-931C-3F2FFF53B7FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>